<commit_message>
new skills for general resume
</commit_message>
<xml_diff>
--- a/skills/skills.xlsx
+++ b/skills/skills.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\resume\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\resume\skills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD695B00-C516-47C6-A5BF-4E7A59757E75}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B729BD2B-F847-4C11-AAC7-C150E7E59428}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="9960" xr2:uid="{552EF8E2-AC39-415A-B2ED-FCF2167AC2C1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$39</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -204,6 +204,27 @@
   </si>
   <si>
     <t>Sysadmin (Linux)</t>
+  </si>
+  <si>
+    <t>Exploit Development</t>
+  </si>
+  <si>
+    <t>Penetration Testing</t>
+  </si>
+  <si>
+    <t>Web Frontend Development</t>
+  </si>
+  <si>
+    <t>Technical Writing</t>
+  </si>
+  <si>
+    <t>soft</t>
+  </si>
+  <si>
+    <t>Technical Leadership</t>
+  </si>
+  <si>
+    <t>Presentation Design &amp; Delivery</t>
   </si>
 </sst>
 </file>
@@ -245,7 +266,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -576,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{943F8701-3D6D-44CA-85C2-82D6A8DC3CC9}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,22 +701,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -644,21 +722,18 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -673,18 +748,18 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -693,10 +768,10 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -704,42 +779,42 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -756,16 +831,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -777,18 +852,21 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -797,10 +875,10 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -808,7 +886,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -834,19 +912,19 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -860,25 +938,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -886,13 +964,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -901,10 +979,10 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -912,13 +990,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -930,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -938,19 +1016,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -964,13 +1042,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -982,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -990,51 +1068,45 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1048,13 +1120,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1063,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1074,13 +1146,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1089,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1100,13 +1175,16 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1115,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1126,7 +1204,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -1135,7 +1213,7 @@
         <v>6</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1144,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -1152,7 +1230,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -1178,19 +1256,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1199,19 +1277,19 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24">
         <v>6</v>
       </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
       <c r="E24">
         <v>0</v>
       </c>
@@ -1219,36 +1297,36 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -1256,42 +1334,42 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1300,44 +1378,44 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1346,27 +1424,30 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1375,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1386,28 +1467,25 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -1415,13 +1493,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1433,18 +1511,18 @@
         <v>0</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D33">
         <v>5</v>
@@ -1459,27 +1537,27 @@
         <v>0</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1488,50 +1566,53 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -1542,89 +1623,280 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D38">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" t="s">
         <v>20</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:G1048576 H1:H39">
+  <autoFilter ref="A1:I39" xr:uid="{8BAF67E4-67E9-4C40-B5E8-BCB0C604F84C}">
+    <sortState ref="A2:I39">
+      <sortCondition ref="C1:C39"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="E1:H42 J42 E46:G1048576 E43:E45">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I42">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43:H43">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:H44">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45:H45">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I39">
+  <conditionalFormatting sqref="I45">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>